<commit_message>
started mirror force and call of hunted
</commit_message>
<xml_diff>
--- a/data/Monster.xlsx
+++ b/data/Monster.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir Ali\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A798214-37AD-40D8-9F2E-7E13D1B7FC79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Monster" sheetId="1" r:id="rId1"/>
+    <sheet name="Monster.xlsx" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -377,28 +372,191 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
-    <font>
-      <sz val="14"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="34">
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -406,112 +564,45 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -523,175 +614,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39998"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -701,33 +805,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -743,7 +820,90 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4" tint="0.49998"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39998"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -758,163 +918,214 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left>
+        <color indexed="0"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right>
+        <color indexed="0"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="61">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="47">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="15"/>
+    <cellStyle name="20% - Accent2" xfId="16"/>
+    <cellStyle name="20% - Accent3" xfId="17"/>
+    <cellStyle name="20% - Accent4" xfId="18"/>
+    <cellStyle name="20% - Accent5" xfId="19"/>
+    <cellStyle name="20% - Accent6" xfId="20"/>
+    <cellStyle name="40% - Accent1" xfId="21"/>
+    <cellStyle name="40% - Accent2" xfId="22"/>
+    <cellStyle name="40% - Accent3" xfId="23"/>
+    <cellStyle name="40% - Accent4" xfId="24"/>
+    <cellStyle name="40% - Accent5" xfId="25"/>
+    <cellStyle name="40% - Accent6" xfId="26"/>
+    <cellStyle name="60% - Accent1" xfId="27"/>
+    <cellStyle name="60% - Accent2" xfId="28"/>
+    <cellStyle name="60% - Accent3" xfId="29"/>
+    <cellStyle name="60% - Accent4" xfId="30"/>
+    <cellStyle name="60% - Accent5" xfId="31"/>
+    <cellStyle name="60% - Accent6" xfId="32"/>
+    <cellStyle name="Accent1" xfId="33"/>
+    <cellStyle name="Accent2" xfId="34"/>
+    <cellStyle name="Accent3" xfId="35"/>
+    <cellStyle name="Accent4" xfId="36"/>
+    <cellStyle name="Accent5" xfId="37"/>
+    <cellStyle name="Accent6" xfId="38"/>
+    <cellStyle name="Bad" xfId="39"/>
+    <cellStyle name="Calculation" xfId="40"/>
+    <cellStyle name="Check Cell" xfId="41"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="43" builtinId="6"/>
+    <cellStyle name="Currency" xfId="44" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="45" builtinId="7"/>
+    <cellStyle name="Explanatory Text" xfId="46"/>
+    <cellStyle name="Good" xfId="47"/>
+    <cellStyle name="Heading 1" xfId="48"/>
+    <cellStyle name="Heading 2" xfId="49"/>
+    <cellStyle name="Heading 3" xfId="50"/>
+    <cellStyle name="Heading 4" xfId="51"/>
+    <cellStyle name="Input" xfId="52"/>
+    <cellStyle name="Linked Cell" xfId="53"/>
+    <cellStyle name="Neutral" xfId="54"/>
+    <cellStyle name="Note" xfId="55"/>
+    <cellStyle name="Output" xfId="56"/>
+    <cellStyle name="Percent" xfId="57" builtinId="5"/>
+    <cellStyle name="Title" xfId="58"/>
+    <cellStyle name="Total" xfId="59"/>
+    <cellStyle name="Warning Text" xfId="60"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -935,7 +1146,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -947,7 +1158,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -994,23 +1205,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1046,23 +1240,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1214,14 +1391,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{2d8d393a-8ef4-427d-b768-881ad8d620ac}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1458,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1487,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1337,7 +1516,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1366,7 +1545,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1395,7 +1574,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1424,7 +1603,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1453,7 +1632,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1482,7 +1661,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1511,7 +1690,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1540,7 +1719,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1569,7 +1748,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1598,7 +1777,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1627,7 +1806,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1656,7 +1835,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1685,7 +1864,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1714,7 +1893,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1743,7 +1922,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1772,7 +1951,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1801,7 +1980,7 @@
         <v>7900</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1830,7 +2009,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1859,7 +2038,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1888,7 +2067,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.25">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1917,7 +2096,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1946,7 +2125,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1975,7 +2154,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2004,7 +2183,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.25">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -2033,7 +2212,7 @@
         <v>9200</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -2062,7 +2241,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2091,7 +2270,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2120,7 +2299,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -2149,7 +2328,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -2178,7 +2357,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14.25">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -2207,7 +2386,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="14.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -2236,7 +2415,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="14.25">
       <c r="A36" t="s">
         <v>101</v>
       </c>
@@ -2265,7 +2444,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.25">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -2294,7 +2473,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14.25">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2323,7 +2502,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -2352,7 +2531,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14.25">
       <c r="A40" t="s">
         <v>109</v>
       </c>
@@ -2381,7 +2560,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="14.25">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -2410,7 +2589,7 @@
         <v>11700</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14.25">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -2440,6 +2619,8 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>